<commit_message>
metabolite keywords from CHEBI
</commit_message>
<xml_diff>
--- a/CMAP_variableMetadata_additions.xlsx
+++ b/CMAP_variableMetadata_additions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\GitHub_niskin\DeepDOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B266056-D3A9-4E2E-99D4-4F531B9A1328}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2051F88-8A59-4305-8C2A-434A9D88A824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28230" yWindow="4635" windowWidth="27000" windowHeight="15030" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25995" yWindow="3825" windowWidth="24090" windowHeight="16605" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="notes" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1179" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1143" uniqueCount="287">
   <si>
     <t>CMAP has some additional metadata they want for each variable measured. There are so many that it makes the most sense to make a separate Excel file and read in the details, no good way to automate this.</t>
   </si>
@@ -2402,8 +2402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2477,9 +2477,6 @@
       <c r="H2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
@@ -2506,9 +2503,6 @@
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
@@ -2535,9 +2529,6 @@
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
@@ -2564,9 +2555,6 @@
       <c r="H5">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
@@ -2593,9 +2581,6 @@
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
@@ -2622,9 +2607,6 @@
       <c r="H7">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" t="s">
@@ -2651,9 +2633,6 @@
       <c r="H8">
         <v>1</v>
       </c>
-      <c r="I8" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9" t="s">
@@ -2680,9 +2659,6 @@
       <c r="H9">
         <v>1</v>
       </c>
-      <c r="I9" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10" t="s">
@@ -2709,9 +2685,6 @@
       <c r="H10">
         <v>1</v>
       </c>
-      <c r="I10" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" t="s">
@@ -2738,9 +2711,6 @@
       <c r="H11">
         <v>1</v>
       </c>
-      <c r="I11" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" t="s">
@@ -2767,9 +2737,6 @@
       <c r="H12">
         <v>1</v>
       </c>
-      <c r="I12" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="13" spans="1:10">
       <c r="A13" t="s">
@@ -2796,9 +2763,6 @@
       <c r="H13">
         <v>1</v>
       </c>
-      <c r="I13" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="14" spans="1:10">
       <c r="A14" t="s">
@@ -2825,9 +2789,6 @@
       <c r="H14">
         <v>1</v>
       </c>
-      <c r="I14" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" t="s">
@@ -2854,9 +2815,6 @@
       <c r="H15">
         <v>1</v>
       </c>
-      <c r="I15" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" t="s">
@@ -2883,11 +2841,8 @@
       <c r="H16">
         <v>1</v>
       </c>
-      <c r="I16" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>105</v>
       </c>
@@ -2912,11 +2867,8 @@
       <c r="H17">
         <v>1</v>
       </c>
-      <c r="I17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -2941,11 +2893,8 @@
       <c r="H18">
         <v>1</v>
       </c>
-      <c r="I18" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" t="s">
         <v>109</v>
       </c>
@@ -2970,11 +2919,8 @@
       <c r="H19">
         <v>1</v>
       </c>
-      <c r="I19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>111</v>
       </c>
@@ -2999,11 +2945,8 @@
       <c r="H20">
         <v>1</v>
       </c>
-      <c r="I20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>113</v>
       </c>
@@ -3028,11 +2971,8 @@
       <c r="H21">
         <v>1</v>
       </c>
-      <c r="I21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -3057,11 +2997,8 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9">
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>117</v>
       </c>
@@ -3086,11 +3023,8 @@
       <c r="H23">
         <v>1</v>
       </c>
-      <c r="I23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9">
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24" t="s">
         <v>119</v>
       </c>
@@ -3115,11 +3049,8 @@
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9">
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>121</v>
       </c>
@@ -3144,11 +3075,8 @@
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9">
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>123</v>
       </c>
@@ -3173,11 +3101,8 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9">
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -3202,11 +3127,8 @@
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9">
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>127</v>
       </c>
@@ -3231,11 +3153,8 @@
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9">
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>129</v>
       </c>
@@ -3260,11 +3179,8 @@
       <c r="H29">
         <v>1</v>
       </c>
-      <c r="I29" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9">
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>131</v>
       </c>
@@ -3289,11 +3205,8 @@
       <c r="H30">
         <v>1</v>
       </c>
-      <c r="I30" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9">
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>133</v>
       </c>
@@ -3318,11 +3231,8 @@
       <c r="H31">
         <v>1</v>
       </c>
-      <c r="I31" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>135</v>
       </c>
@@ -3347,11 +3257,8 @@
       <c r="H32">
         <v>1</v>
       </c>
-      <c r="I32" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>137</v>
       </c>
@@ -3376,11 +3283,8 @@
       <c r="H33">
         <v>1</v>
       </c>
-      <c r="I33" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9">
+    </row>
+    <row r="34" spans="1:8">
       <c r="A34" t="s">
         <v>139</v>
       </c>
@@ -3405,11 +3309,8 @@
       <c r="H34">
         <v>1</v>
       </c>
-      <c r="I34" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>141</v>
       </c>
@@ -3434,11 +3335,8 @@
       <c r="H35">
         <v>1</v>
       </c>
-      <c r="I35" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
+    </row>
+    <row r="36" spans="1:8">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -3463,11 +3361,8 @@
       <c r="H36">
         <v>1</v>
       </c>
-      <c r="I36" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>145</v>
       </c>
@@ -3491,9 +3386,6 @@
       </c>
       <c r="H37">
         <v>1</v>
-      </c>
-      <c r="I37" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -5339,7 +5231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>

</xml_diff>